<commit_message>
Final Update, Documentation and Mastering
</commit_message>
<xml_diff>
--- a/documentation/Asset_List.xlsx
+++ b/documentation/Asset_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eiz17\Desktop\Interactive Game Audio\671_Final_Project\671_Final_Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463C7660-751B-44E5-830C-DAD0549A0A7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5051E5B5-0FB4-40CA-9549-EFA6D855C110}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4956" yWindow="3288" windowWidth="17280" windowHeight="8964" xr2:uid="{C79EB596-7827-4FD9-89C3-C7F7EBB96D27}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>Description</t>
   </si>
@@ -54,9 +54,6 @@
     <t>UI Sound</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Watering</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Select_Tile</t>
   </si>
   <si>
-    <t>Background ambience that plays throughout the game. Louder during menus, contains bird chirps, wind whistling, dog bark, windchimes, bugs buzzing, etc</t>
-  </si>
-  <si>
     <t>Sound that plays when a tile is selected - method that gives info on tiles. Dirt crunching sound (potentially more based on different tile types, I don’t want to overscope)</t>
   </si>
   <si>
@@ -157,6 +151,15 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Title_Ambience</t>
+  </si>
+  <si>
+    <t>Scatterer instrument that plays in the title screen</t>
+  </si>
+  <si>
+    <t>Background ambience that plays throughout the game. Quieter during menus, contains bird chirps, wind whistling, dog bark, windchimes, bugs buzzing, etc</t>
   </si>
 </sst>
 </file>
@@ -528,15 +531,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EDD1CBE-E29A-4DDA-8CF4-464F2FCEEF86}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="139.5546875" bestFit="1" customWidth="1"/>
@@ -544,7 +548,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -570,185 +574,185 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -757,27 +761,44 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
         <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>